<commit_message>
update 1 RC 1
</commit_message>
<xml_diff>
--- a/testplan.xlsx
+++ b/testplan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>size of stamps</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>touch up outside canvas</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>restore from clean install</t>
+  </si>
+  <si>
+    <t>thumbs</t>
+  </si>
+  <si>
+    <t>splashes</t>
   </si>
 </sst>
 </file>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D7"/>
+  <dimension ref="A3:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -450,6 +462,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>